<commit_message>
base map done, utility functions added, global setting completed
</commit_message>
<xml_diff>
--- a/Data_Conversion.xlsx
+++ b/Data_Conversion.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zq/Desktop/InProgress-Hwy-Simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547C2260-3723-1A45-8891-3C91E0E8F18E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAD0C1A-9BF8-564A-A876-7BA133A55036}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8440" yWindow="460" windowWidth="19980" windowHeight="17040" xr2:uid="{E0E0BC84-8A9D-A04D-A89C-7F4722BDBB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +231,14 @@
       <i/>
       <sz val="13"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,6 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEFF62DB-C855-1446-98D2-24A732CB0282}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J5" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,7 +986,7 @@
       <c r="L23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="26" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>